<commit_message>
update results in excel file
</commit_message>
<xml_diff>
--- a/Wyniki_klasyfikacji.xlsx
+++ b/Wyniki_klasyfikacji.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\PycharmProjects\Blog_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84B2192-411B-42A5-ADA9-A8D153C7C9E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E67937-0FDB-465D-97E9-6AA321FA8B30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9AE33677-8FE6-440E-A34E-B325EF81A99F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>Model</t>
   </si>
@@ -160,6 +160,9 @@
   <si>
     <t>NB</t>
   </si>
+  <si>
+    <t>XGB</t>
+  </si>
 </sst>
 </file>
 
@@ -167,7 +170,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -229,7 +232,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -548,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654458F8-16C9-484F-BD19-52933573A6C8}">
-  <dimension ref="B3:E29"/>
+  <dimension ref="B3:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -678,7 +681,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:6">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -692,7 +695,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:6">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -706,12 +709,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:6">
       <c r="B22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:6">
       <c r="B23" t="s">
         <v>24</v>
       </c>
@@ -719,7 +722,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:6">
       <c r="B24" t="s">
         <v>25</v>
       </c>
@@ -727,7 +730,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:6">
       <c r="B25" t="s">
         <v>23</v>
       </c>
@@ -740,8 +743,11 @@
       <c r="E25">
         <v>10000</v>
       </c>
-    </row>
-    <row r="26" spans="2:5">
+      <c r="F25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
       <c r="B26" t="s">
         <v>17</v>
       </c>
@@ -754,8 +760,11 @@
       <c r="E26" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="2:5">
+      <c r="F26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
       <c r="B27" t="s">
         <v>27</v>
       </c>
@@ -768,8 +777,11 @@
       <c r="E27">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="2:5">
+      <c r="F27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
       <c r="B28" t="s">
         <v>20</v>
       </c>
@@ -782,8 +794,11 @@
       <c r="E28">
         <v>0.63400000000000001</v>
       </c>
-    </row>
-    <row r="29" spans="2:5">
+      <c r="F28">
+        <v>0.59699999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6">
       <c r="B29" t="s">
         <v>21</v>
       </c>
@@ -795,6 +810,9 @@
       </c>
       <c r="E29">
         <v>0.63300000000000001</v>
+      </c>
+      <c r="F29">
+        <v>0.60799999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>